<commit_message>
changes from the client(journal entries, reports, export to excel)
</commit_message>
<xml_diff>
--- a/public/extra/export_report/export_report_template_journal.xlsx
+++ b/public/extra/export_report/export_report_template_journal.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>SPECIFIC DATE</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>CHECK VOUCHER NO.</t>
   </si>
   <si>
@@ -35,9 +32,6 @@
   </si>
   <si>
     <t>CLASSIFICATION</t>
-  </si>
-  <si>
-    <t>OT/IT</t>
   </si>
   <si>
     <t>DR</t>
@@ -482,28 +476,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:Q4"/>
+  <dimension ref="B4:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -516,28 +510,22 @@
         <v>7</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small adjustment in journal entry
</commit_message>
<xml_diff>
--- a/public/extra/export_report/export_report_template_journal.xlsx
+++ b/public/extra/export_report/export_report_template_journal.xlsx
@@ -19,12 +19,6 @@
     <t>SPECIFIC DATE</t>
   </si>
   <si>
-    <t>CHECK VOUCHER NO.</t>
-  </si>
-  <si>
-    <t>JOURNAL VOUCHER NO.</t>
-  </si>
-  <si>
     <t>CHART CODE</t>
   </si>
   <si>
@@ -56,6 +50,12 @@
   </si>
   <si>
     <t>REFERENCE NUMBER</t>
+  </si>
+  <si>
+    <t>JV NO.</t>
+  </si>
+  <si>
+    <t>CV NO.</t>
   </si>
 </sst>
 </file>
@@ -479,53 +479,53 @@
   <dimension ref="B4:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="M4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>